<commit_message>
Feature: finish NS 100 (issue #3345)
</commit_message>
<xml_diff>
--- a/docs/cost_factors.xlsx
+++ b/docs/cost_factors.xlsx
@@ -4,20 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
+    <sheet name="electric" sheetId="1" r:id="rId1"/>
+    <sheet name="diesel" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Blad1!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">diesel!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">electric!$E$3</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>SH '30'</t>
   </si>
@@ -97,6 +103,18 @@
   </si>
   <si>
     <t>multiplier</t>
+  </si>
+  <si>
+    <t>SH/Hendry '25'</t>
+  </si>
+  <si>
+    <t>UU '37'</t>
+  </si>
+  <si>
+    <t>Floss '47'</t>
+  </si>
+  <si>
+    <t>SH '125'</t>
   </si>
 </sst>
 </file>
@@ -447,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,24 +750,295 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0.15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <v>128</v>
+      </c>
+      <c r="F10">
+        <v>1267</v>
+      </c>
+      <c r="G10">
+        <v>213</v>
+      </c>
+      <c r="H10">
+        <v>18</v>
+      </c>
+      <c r="I10">
+        <v>17578</v>
+      </c>
+      <c r="J10">
+        <f>I10*$J$17/$I$17</f>
+        <v>15.001137872179026</v>
+      </c>
+      <c r="K10">
+        <f>(D10*$E$3+SQRT(F10)*$E$4+H10*$E$5)/$E$6</f>
+        <v>28.678483038334612</v>
+      </c>
+      <c r="L10">
+        <v>1267</v>
+      </c>
+      <c r="M10">
+        <f>L10*$M$17/$L$17</f>
+        <v>83.218390804597703</v>
+      </c>
+      <c r="N10" s="2">
+        <f>(E10*$H$3+SQRT(F10)*$H$4)/$H$6</f>
+        <v>25.617724557501916</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>101</v>
+      </c>
+      <c r="E11">
+        <v>144</v>
+      </c>
+      <c r="F11">
+        <v>1774</v>
+      </c>
+      <c r="G11">
+        <v>299</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <v>19921</v>
+      </c>
+      <c r="J11">
+        <f>I11*$J$17/$I$17</f>
+        <v>17.000663758771097</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K13" si="0">(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5)/$E$6</f>
+        <v>34.735663813191614</v>
+      </c>
+      <c r="L11">
+        <v>1828</v>
+      </c>
+      <c r="M11">
+        <f>L11*$M$17/$L$17</f>
+        <v>120.0656814449918</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11:N13" si="1">(E11*$H$3+SQRT(F11)*$H$4)/$H$6</f>
+        <v>29.753495719787416</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>160</v>
+      </c>
+      <c r="F12">
+        <v>2616</v>
+      </c>
+      <c r="G12">
+        <v>332</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <v>21093</v>
+      </c>
+      <c r="J12">
+        <f>I12*$J$17/$I$17</f>
+        <v>18.000853404134268</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>39.744054223053311</v>
+      </c>
+      <c r="L12">
+        <v>2132</v>
+      </c>
+      <c r="M12">
+        <f>L12*$M$17/$L$17</f>
+        <v>140.03284072249591</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>35.016081334579958</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>140</v>
+      </c>
+      <c r="E13">
+        <v>201</v>
+      </c>
+      <c r="F13">
+        <v>4563</v>
+      </c>
+      <c r="G13">
+        <v>415</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>23437</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>46.264994448555868</v>
+      </c>
+      <c r="L13">
+        <v>2894</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="1"/>
+        <v>45.472491672833797</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>5273</v>
+      </c>
+      <c r="J17">
+        <v>4.5</v>
+      </c>
+      <c r="L17">
+        <v>609</v>
+      </c>
+      <c r="M17">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature: finish GVB M1M2 (issue #2951, issue #3345)
</commit_message>
<xml_diff>
--- a/docs/cost_factors.xlsx
+++ b/docs/cost_factors.xlsx
@@ -4,34 +4,50 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="electric" sheetId="1" r:id="rId1"/>
     <sheet name="diesel" sheetId="4" r:id="rId2"/>
+    <sheet name="dmu" sheetId="5" r:id="rId3"/>
+    <sheet name="metro" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">diesel!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">dmu!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">electric!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">metro!$E$3</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
   <si>
     <t>SH '30'</t>
   </si>
@@ -115,6 +131,18 @@
   </si>
   <si>
     <t>SH '125'</t>
+  </si>
+  <si>
+    <t>manley-More DMU</t>
+  </si>
+  <si>
+    <t>Dash'</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>capacity_coeff</t>
   </si>
 </sst>
 </file>
@@ -158,10 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -752,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,4 +1070,474 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0.15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>112</v>
+      </c>
+      <c r="F11">
+        <v>608</v>
+      </c>
+      <c r="G11">
+        <v>190</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>76</v>
+      </c>
+      <c r="J11">
+        <v>12890</v>
+      </c>
+      <c r="K11">
+        <f>J11*$K$18/$J$18</f>
+        <v>11.000379290726341</v>
+      </c>
+      <c r="L11">
+        <f>(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5+I11*$E$6)/$E$7</f>
+        <v>23.797296803562773</v>
+      </c>
+      <c r="M11">
+        <v>1294</v>
+      </c>
+      <c r="N11">
+        <f>M11*$N$18/$M$18</f>
+        <v>84.991789819376024</v>
+      </c>
+      <c r="O11" s="2">
+        <f>(E11*$H$3+SQRT(F11)*$H$4+I11*$H$6)/$H$7</f>
+        <v>19.263062404750364</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>710</v>
+      </c>
+      <c r="G12">
+        <v>225</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>80</v>
+      </c>
+      <c r="J12">
+        <v>16406</v>
+      </c>
+      <c r="K12">
+        <f>J12*$K$18/$J$18</f>
+        <v>14.000948226815854</v>
+      </c>
+      <c r="L12">
+        <f>(D12*$E$3+SQRT(F12)*$E$4+H12*$E$5+I12*$E$6)/$E$7</f>
+        <v>26.593747556684537</v>
+      </c>
+      <c r="M12">
+        <v>1066</v>
+      </c>
+      <c r="N12">
+        <f>M12*$N$18/$M$18</f>
+        <v>70.016420361247953</v>
+      </c>
+      <c r="O12" s="2">
+        <f>(E12*$H$3+SQRT(F12)*$H$4+I12*$H$6)/$H$7</f>
+        <v>20.658330075579386</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>5273</v>
+      </c>
+      <c r="K18">
+        <v>4.5</v>
+      </c>
+      <c r="M18">
+        <v>609</v>
+      </c>
+      <c r="N18">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:O18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0.15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>112</v>
+      </c>
+      <c r="F11">
+        <v>608</v>
+      </c>
+      <c r="G11">
+        <v>190</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>76</v>
+      </c>
+      <c r="J11">
+        <v>12890</v>
+      </c>
+      <c r="K11">
+        <f>J11*$K$18/$J$18</f>
+        <v>10.999466666666667</v>
+      </c>
+      <c r="L11">
+        <f>(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5+I11*$E$6)/$E$7</f>
+        <v>11.898648401781386</v>
+      </c>
+      <c r="M11">
+        <v>1294</v>
+      </c>
+      <c r="N11">
+        <f>M11*$N$18/$M$18</f>
+        <v>92.09964412811388</v>
+      </c>
+      <c r="O11" s="2">
+        <f>(E11*$H$3+SQRT(F11)*$H$4+I11*$H$6)/$H$7</f>
+        <v>84.652249619001452</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>710</v>
+      </c>
+      <c r="G12">
+        <v>225</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>80</v>
+      </c>
+      <c r="J12">
+        <v>16406</v>
+      </c>
+      <c r="K12">
+        <f>J12*$K$18/$J$18</f>
+        <v>13.999786666666667</v>
+      </c>
+      <c r="L12">
+        <f>(D12*$E$3+SQRT(F12)*$E$4+H12*$E$5+I12*$E$6)/$E$7</f>
+        <v>13.296873778342269</v>
+      </c>
+      <c r="M12">
+        <v>1066</v>
+      </c>
+      <c r="N12">
+        <f>M12*$N$18/$M$18</f>
+        <v>75.871886120996436</v>
+      </c>
+      <c r="O12" s="2">
+        <f>(E12*$H$3+SQRT(F12)*$H$4+I12*$H$6)/$H$7</f>
+        <v>90.633320302317543</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>243750</v>
+      </c>
+      <c r="K18">
+        <v>208</v>
+      </c>
+      <c r="M18">
+        <v>562</v>
+      </c>
+      <c r="N18">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feature: finish NS 3900 (issue #3345)
</commit_message>
<xml_diff>
--- a/docs/cost_factors.xlsx
+++ b/docs/cost_factors.xlsx
@@ -9,45 +9,53 @@
   <sheets>
     <sheet name="electric" sheetId="1" r:id="rId1"/>
     <sheet name="diesel" sheetId="4" r:id="rId2"/>
-    <sheet name="dmu" sheetId="5" r:id="rId3"/>
-    <sheet name="metro" sheetId="6" r:id="rId4"/>
+    <sheet name="steam" sheetId="7" r:id="rId3"/>
+    <sheet name="dmu" sheetId="5" r:id="rId4"/>
+    <sheet name="metro" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">diesel!$E$3</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">dmu!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">dmu!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">electric!$E$3</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">metro!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">metro!$E$3</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">steam!$E$3</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="36">
   <si>
     <t>SH '30'</t>
   </si>
@@ -143,6 +151,18 @@
   </si>
   <si>
     <t>capacity_coeff</t>
+  </si>
+  <si>
+    <t>Kirby Paul Tank</t>
+  </si>
+  <si>
+    <t>Chaney 'Jubilee'</t>
+  </si>
+  <si>
+    <t>Ginzu 'A4'</t>
+  </si>
+  <si>
+    <t>SH '8P'</t>
   </si>
 </sst>
 </file>
@@ -1074,9 +1094,312 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>47</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>304</v>
+      </c>
+      <c r="G10">
+        <v>139</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>8203</v>
+      </c>
+      <c r="J10">
+        <f>I10*$J$17/$I$17</f>
+        <v>7.0004741134079271</v>
+      </c>
+      <c r="K10">
+        <f>(D10*$E$3+SQRT(F10)*$E$4+H10*$E$5)/$E$6</f>
+        <v>14.38711915483254</v>
+      </c>
+      <c r="L10">
+        <v>820</v>
+      </c>
+      <c r="M10">
+        <f>L10*$M$17/$L$17</f>
+        <v>50</v>
+      </c>
+      <c r="N10" s="2">
+        <f>(E10*$H$3+SQRT(F10)*$H$4)/$H$6</f>
+        <v>14.246018098373213</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>131</v>
+      </c>
+      <c r="E11">
+        <v>112</v>
+      </c>
+      <c r="F11">
+        <v>1014</v>
+      </c>
+      <c r="G11">
+        <v>388</v>
+      </c>
+      <c r="H11">
+        <v>21</v>
+      </c>
+      <c r="I11">
+        <v>15234</v>
+      </c>
+      <c r="J11">
+        <f>I11*$J$17/$I$17</f>
+        <v>13.000758581452683</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K13" si="0">(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5)/$E$6</f>
+        <v>34.66867333123627</v>
+      </c>
+      <c r="L11">
+        <v>1968</v>
+      </c>
+      <c r="M11">
+        <f>L11*$M$17/$L$17</f>
+        <v>120</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11:N13" si="1">(E11*$H$3+SQRT(F11)*$H$4)/$H$6</f>
+        <v>25.529514995281595</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>162</v>
+      </c>
+      <c r="E12">
+        <v>128</v>
+      </c>
+      <c r="F12">
+        <v>1217</v>
+      </c>
+      <c r="G12">
+        <v>480</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>22265</v>
+      </c>
+      <c r="J12">
+        <f>I12*$J$17/$I$17</f>
+        <v>19.00104304949744</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>41.377105417004962</v>
+      </c>
+      <c r="L12">
+        <v>2296</v>
+      </c>
+      <c r="M12">
+        <f>L12*$M$17/$L$17</f>
+        <v>140</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>28.498487188261169</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>170</v>
+      </c>
+      <c r="E13">
+        <v>144</v>
+      </c>
+      <c r="F13">
+        <v>1622</v>
+      </c>
+      <c r="G13">
+        <v>504</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>25781</v>
+      </c>
+      <c r="J13">
+        <f>I13*$J$17/$I$17</f>
+        <v>22.001611985586951</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13" si="2">(D13*$E$3+SQRT(F13)*$E$4+H13*$E$5)/$E$6</f>
+        <v>44.354812226240902</v>
+      </c>
+      <c r="L13">
+        <v>2132</v>
+      </c>
+      <c r="M13">
+        <f>L13*$M$17/$L$17</f>
+        <v>130</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" ref="N13" si="3">(E13*$H$3+SQRT(F13)*$H$4)/$H$6</f>
+        <v>32.523327509042041</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>5273</v>
+      </c>
+      <c r="J17">
+        <v>4.5</v>
+      </c>
+      <c r="L17">
+        <v>656</v>
+      </c>
+      <c r="M17">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1307,7 +1630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:O18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Feature: finish HS-DD coach (issue #2951, issue #3345)
</commit_message>
<xml_diff>
--- a/docs/cost_factors.xlsx
+++ b/docs/cost_factors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="electric" sheetId="1" r:id="rId1"/>
@@ -12,38 +12,46 @@
     <sheet name="steam" sheetId="7" r:id="rId3"/>
     <sheet name="dmu" sheetId="5" r:id="rId4"/>
     <sheet name="metro" sheetId="6" r:id="rId5"/>
+    <sheet name="coaches" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">coaches!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">diesel!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">dmu!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">electric!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">metro!$E$3</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">steam!$E$3</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="38">
   <si>
     <t>SH '30'</t>
   </si>
@@ -163,6 +171,12 @@
   </si>
   <si>
     <t>SH '8P'</t>
+  </si>
+  <si>
+    <t>running_cost_diesel</t>
+  </si>
+  <si>
+    <t>passenger carriage</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1271,7 +1285,7 @@
         <v>13.000758581452683</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K13" si="0">(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5)/$E$6</f>
+        <f t="shared" ref="K11:K12" si="0">(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5)/$E$6</f>
         <v>34.66867333123627</v>
       </c>
       <c r="L11">
@@ -1282,7 +1296,7 @@
         <v>120</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" ref="N11:N13" si="1">(E11*$H$3+SQRT(F11)*$H$4)/$H$6</f>
+        <f t="shared" ref="N11:N12" si="1">(E11*$H$3+SQRT(F11)*$H$4)/$H$6</f>
         <v>25.529514995281595</v>
       </c>
     </row>
@@ -1863,4 +1877,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2.4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>1.6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>160</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>1447</v>
+      </c>
+      <c r="K11">
+        <f>J11*$K$18/$J$18</f>
+        <v>123.56069958847736</v>
+      </c>
+      <c r="L11">
+        <f>(D11*$E$3+SQRT(F11)*$E$4+H11*$E$5+I11*$E$6)/$E$7</f>
+        <v>62</v>
+      </c>
+      <c r="M11">
+        <f>J11/8</f>
+        <v>180.875</v>
+      </c>
+      <c r="N11">
+        <f>M11*$N$18/$M$18</f>
+        <v>11.880131362889983</v>
+      </c>
+      <c r="O11" s="2">
+        <f>(E11*$H$3+SQRT(F11)*$H$4+I11*$H$6)/$H$7</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="3"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>972</v>
+      </c>
+      <c r="K18">
+        <v>83</v>
+      </c>
+      <c r="M18">
+        <v>609</v>
+      </c>
+      <c r="N18">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>